<commit_message>
First py ta fm
</commit_message>
<xml_diff>
--- a/Controller/Controller_Module1.xlsx
+++ b/Controller/Controller_Module1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationFramework\Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78E6AAA-CC6C-41AD-9677-7A826D328D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95318AC5-06EA-4873-AA77-FF9763AD9579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6B930F6A-1585-46EA-8B3E-7080AD777EC1}"/>
   </bookViews>
@@ -56,15 +56,9 @@
     <t>TestDataSet</t>
   </si>
   <si>
-    <t>TC001 SearchInJioMart</t>
-  </si>
-  <si>
     <t>taasframework.com.qa.test.JioMart</t>
   </si>
   <si>
-    <t xml:space="preserve">Search Item in Jio mart </t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -78,6 +72,12 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>TC001 TestCase_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Case 1 </t>
   </si>
 </sst>
 </file>
@@ -531,7 +531,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,22 +567,22 @@
     <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="str">
         <f>CONCATENATE("TC_",SUBSTITUTE(B2," ","_"))</f>
-        <v>TC_TC001_SearchInJioMart</v>
+        <v>TC_TC001_TestCase_001</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -591,19 +591,19 @@
         <v>TC_TC002_DoSomething</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="F3" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>